<commit_message>
Atualizações após dados finais recebidos
O professor enviou os últimos dados em 24/03/2025.
</commit_message>
<xml_diff>
--- a/docs/AIP2025 - minissimpósios.xlsx
+++ b/docs/AIP2025 - minissimpósios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmilson1\Documents\UFSC\Pós-graduação em Engenharia de Automação e Sistemas - informal\MIP WAY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85662F3-FD1C-4218-B84E-CEFD4EE02A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FE165A-8628-43F0-ADB2-EE9687566A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{437734A5-5378-4F16-8D0F-8872D35B0FF6}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{437734A5-5378-4F16-8D0F-8872D35B0FF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +124,30 @@
   </si>
   <si>
     <t>MS-30</t>
+  </si>
+  <si>
+    <t>MS-31</t>
+  </si>
+  <si>
+    <t>MS-32</t>
+  </si>
+  <si>
+    <t>MS-33</t>
+  </si>
+  <si>
+    <t>MS-34</t>
+  </si>
+  <si>
+    <t>MS-35</t>
+  </si>
+  <si>
+    <t>MS-36</t>
+  </si>
+  <si>
+    <t>MS-37</t>
+  </si>
+  <si>
+    <t>MS-38</t>
   </si>
 </sst>
 </file>
@@ -514,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E2E5DD-C727-4EA0-80BC-09BB8EF9DD2D}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C2" sqref="C2:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +680,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -667,7 +691,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -865,6 +889,94 @@
         <v>32</v>
       </c>
       <c r="C31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39">
         <v>2</v>
       </c>
     </row>

</xml_diff>